<commit_message>
Feat - gamelogic construction
</commit_message>
<xml_diff>
--- a/doc/slots and signals.xlsx
+++ b/doc/slots and signals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yvan.denis\Documents\QtProject\snake\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{081A9979-97FD-484F-8B3E-CC8358D144BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C987CA5-D45B-45C6-BCBE-F2B96D8E3C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="1110" windowWidth="29040" windowHeight="15255" xr2:uid="{1C28437B-6A45-4904-8BCA-DFF0A4B37255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C28437B-6A45-4904-8BCA-DFF0A4B37255}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>slots</t>
   </si>
@@ -94,13 +94,25 @@
   </si>
   <si>
     <t>maindows</t>
+  </si>
+  <si>
+    <t>startGame</t>
+  </si>
+  <si>
+    <t>gameWidget</t>
+  </si>
+  <si>
+    <t>statwidget</t>
+  </si>
+  <si>
+    <t>stopGame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +133,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF800000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00677C"/>
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
@@ -144,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,12 +175,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +502,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B4" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -507,61 +528,81 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8" t="s">
+        <v>2</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -633,7 +674,7 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -650,7 +691,7 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
@@ -668,7 +709,7 @@
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="1"/>
@@ -683,7 +724,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -693,8 +734,8 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -704,8 +745,8 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -737,11 +778,12 @@
       <c r="I23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B4:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>